<commit_message>
l,r & pre if short zeropaf
</commit_message>
<xml_diff>
--- a/Python/Comments_L.xlsx
+++ b/Python/Comments_L.xlsx
@@ -5,7 +5,7 @@
   <workbookPr defaultThemeVersion="164011"/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
-      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\LeeJiWon\Desktop\OpenBCI\AAD\Python\"/>
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\user\Desktop\hy-kist\OpenBCI\AAD\Python\"/>
     </mc:Choice>
   </mc:AlternateContent>
   <bookViews>
@@ -24,7 +24,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="46" uniqueCount="46">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="47" uniqueCount="47">
   <si>
     <t>Num</t>
     <phoneticPr fontId="1" type="noConversion"/>
@@ -127,11 +127,6 @@
     <phoneticPr fontId="1" type="noConversion"/>
   </si>
   <si>
-    <t>세션 2
-'스페이스 바' 를 누르시면 세션 2 시작합니다.</t>
-    <phoneticPr fontId="1" type="noConversion"/>
-  </si>
-  <si>
     <t>세션 3
 세션 3에서는 총 6쌍의 이야기가 제시되며, 예상 소요 시간은 약 7분입니다.
 참여자분께서는 6개의 이야기 쌍 중 
@@ -167,11 +162,6 @@
 소요시간은 약 7분 정도입니다.
 음성 자극이 제시되는 동안은 몸의 움직임을 가능한 최소화해주시고,
 시선은 화면 중앙에 고정해주시길 바랍니다.</t>
-    <phoneticPr fontId="1" type="noConversion"/>
-  </si>
-  <si>
-    <t>세션 4
-'스페이스 바' 를 누르시면 세션 4 시작합니다.</t>
     <phoneticPr fontId="1" type="noConversion"/>
   </si>
   <si>
@@ -219,11 +209,6 @@
     <phoneticPr fontId="1" type="noConversion"/>
   </si>
   <si>
-    <t>세션 5
-'스페이스 바' 를 누르시면 세션 5 시작합니다.</t>
-    <phoneticPr fontId="1" type="noConversion"/>
-  </si>
-  <si>
     <t>예를 들어, 왼쪽에 제시되는 이야기에 주의를 기울여야 하는 경우,
 이야기 쌍이 제시되기 전, 왼쪽 귀에 '삐- 삐-'라는 신호음이 들릴 것입니다.
 동시에 모니터 화면 중앙에는 왼쪽 방향을 가리키는 화살표 '&lt;&lt;&lt;' 가 제시됩니다.
@@ -296,11 +281,6 @@
     <phoneticPr fontId="1" type="noConversion"/>
   </si>
   <si>
-    <t>세션 1
-'스페이스 바' 를 누르시면 세션 1 시작합니다.</t>
-    <phoneticPr fontId="1" type="noConversion"/>
-  </si>
-  <si>
     <t xml:space="preserve">각 세션 별로 주의를 기울여야 하는 방향이 다릅니다.
 '세션 1' 에서는 "왼쪽"으로 제시되는 이야기에 집중하셔야 합니다.
 '세션 2' 에서는 "오른쪽"으로 제시되는 이야기에 집중하셔야 합니다.
@@ -351,6 +331,31 @@
 정답률 80% 미만을 달성하신 분의 뇌파 데이터는 
 이후 분석 과정에 포함될 수 없기에 사례비는 차감 지급되오니
 집중하여 들어주시기 바랍니다.</t>
+    <phoneticPr fontId="1" type="noConversion"/>
+  </si>
+  <si>
+    <t>세션 1
+'스페이스 바' 를 누르시면 세션 1 이 시작됩니다.</t>
+    <phoneticPr fontId="1" type="noConversion"/>
+  </si>
+  <si>
+    <t>세션 3
+'스페이스 바' 를 누르시면 세션 3 이 시작됩니다.</t>
+    <phoneticPr fontId="1" type="noConversion"/>
+  </si>
+  <si>
+    <t>세션 4
+'스페이스 바' 를 누르시면 세션 4 가 시작됩니다.</t>
+    <phoneticPr fontId="1" type="noConversion"/>
+  </si>
+  <si>
+    <t>세션 5
+'스페이스 바' 를 누르시면 세션 5 가 시작됩니다.</t>
+    <phoneticPr fontId="1" type="noConversion"/>
+  </si>
+  <si>
+    <t>세션 2
+'스페이스 바' 를 누르시면 세션 2 가 시작됩니다.</t>
     <phoneticPr fontId="1" type="noConversion"/>
   </si>
 </sst>
@@ -713,8 +718,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <dimension ref="A1:H12"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="A6" zoomScale="50" zoomScaleNormal="50" workbookViewId="0">
-      <selection activeCell="B8" sqref="B8"/>
+    <sheetView tabSelected="1" topLeftCell="A4" zoomScale="50" zoomScaleNormal="50" workbookViewId="0">
+      <selection activeCell="D5" sqref="D5"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="17.399999999999999" x14ac:dyDescent="0.4"/>
@@ -765,16 +770,16 @@
         <v>10</v>
       </c>
       <c r="D2" s="1" t="s">
-        <v>35</v>
+        <v>32</v>
       </c>
       <c r="E2" s="1" t="s">
-        <v>19</v>
+        <v>18</v>
       </c>
       <c r="F2" s="1" t="s">
-        <v>36</v>
+        <v>33</v>
       </c>
       <c r="G2" s="1" t="s">
-        <v>43</v>
+        <v>39</v>
       </c>
     </row>
     <row r="3" spans="1:8" ht="261" x14ac:dyDescent="0.4">
@@ -791,13 +796,13 @@
         <v>14</v>
       </c>
       <c r="E3" s="4" t="s">
-        <v>17</v>
+        <v>16</v>
       </c>
       <c r="F3" s="2" t="s">
-        <v>20</v>
+        <v>19</v>
       </c>
       <c r="G3" s="2" t="s">
-        <v>23</v>
+        <v>21</v>
       </c>
     </row>
     <row r="4" spans="1:8" ht="348" x14ac:dyDescent="0.4">
@@ -805,7 +810,7 @@
         <v>3</v>
       </c>
       <c r="B4" s="2" t="s">
-        <v>44</v>
+        <v>40</v>
       </c>
       <c r="C4" s="2" t="s">
         <v>12</v>
@@ -814,13 +819,13 @@
         <v>15</v>
       </c>
       <c r="E4" s="4" t="s">
-        <v>18</v>
+        <v>17</v>
       </c>
       <c r="F4" s="4" t="s">
-        <v>21</v>
+        <v>20</v>
       </c>
       <c r="G4" s="2" t="s">
-        <v>24</v>
+        <v>22</v>
       </c>
     </row>
     <row r="5" spans="1:8" ht="365.4" x14ac:dyDescent="0.4">
@@ -828,31 +833,33 @@
         <v>4</v>
       </c>
       <c r="B5" s="2" t="s">
-        <v>29</v>
+        <v>26</v>
       </c>
       <c r="C5" s="2" t="s">
-        <v>39</v>
+        <v>35</v>
       </c>
       <c r="D5" s="5" t="s">
-        <v>16</v>
-      </c>
-      <c r="E5" s="5"/>
+        <v>46</v>
+      </c>
+      <c r="E5" s="5" t="s">
+        <v>43</v>
+      </c>
       <c r="F5" s="5" t="s">
-        <v>22</v>
+        <v>44</v>
       </c>
       <c r="G5" s="2" t="s">
-        <v>37</v>
+        <v>34</v>
       </c>
     </row>
     <row r="6" spans="1:8" ht="243.6" x14ac:dyDescent="0.4">
       <c r="B6" s="3" t="s">
-        <v>31</v>
+        <v>28</v>
       </c>
       <c r="C6" s="2" t="s">
-        <v>41</v>
+        <v>37</v>
       </c>
       <c r="G6" s="2" t="s">
-        <v>25</v>
+        <v>23</v>
       </c>
     </row>
     <row r="7" spans="1:8" ht="409.6" x14ac:dyDescent="0.4">
@@ -860,13 +867,13 @@
         <v>5</v>
       </c>
       <c r="B7" s="2" t="s">
-        <v>32</v>
+        <v>29</v>
       </c>
       <c r="C7" s="1" t="s">
-        <v>40</v>
+        <v>36</v>
       </c>
       <c r="G7" s="2" t="s">
-        <v>26</v>
+        <v>24</v>
       </c>
     </row>
     <row r="8" spans="1:8" ht="208.8" x14ac:dyDescent="0.4">
@@ -874,13 +881,13 @@
         <v>6</v>
       </c>
       <c r="B8" s="2" t="s">
-        <v>45</v>
+        <v>41</v>
       </c>
       <c r="C8" s="2" t="s">
         <v>13</v>
       </c>
       <c r="G8" s="4" t="s">
-        <v>27</v>
+        <v>25</v>
       </c>
     </row>
     <row r="9" spans="1:8" ht="174" x14ac:dyDescent="0.4">
@@ -888,13 +895,13 @@
         <v>7</v>
       </c>
       <c r="B9" s="2" t="s">
-        <v>30</v>
+        <v>27</v>
       </c>
       <c r="C9" s="2" t="s">
-        <v>42</v>
+        <v>38</v>
       </c>
       <c r="G9" s="5" t="s">
-        <v>28</v>
+        <v>45</v>
       </c>
     </row>
     <row r="10" spans="1:8" ht="261" x14ac:dyDescent="0.4">
@@ -902,17 +909,17 @@
         <v>8</v>
       </c>
       <c r="C10" s="2" t="s">
-        <v>33</v>
+        <v>30</v>
       </c>
     </row>
     <row r="11" spans="1:8" ht="174" x14ac:dyDescent="0.4">
       <c r="C11" s="4" t="s">
-        <v>34</v>
+        <v>31</v>
       </c>
     </row>
     <row r="12" spans="1:8" ht="69.599999999999994" x14ac:dyDescent="0.4">
       <c r="C12" s="5" t="s">
-        <v>38</v>
+        <v>42</v>
       </c>
     </row>
   </sheetData>

</xml_diff>